<commit_message>
Update order of services in programs
</commit_message>
<xml_diff>
--- a/documents/Install Notes.xlsx
+++ b/documents/Install Notes.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\MinimalOcelot\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698A1495-C4D9-40E1-9E81-037C1CF59C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FA9D5B-340D-4315-8290-84EFB0D163E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="1236" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{31A6B894-E528-4D1F-99B7-355F9E47661B}"/>
+    <workbookView xWindow="22944" yWindow="1248" windowWidth="23232" windowHeight="12696" activeTab="2" xr2:uid="{31A6B894-E528-4D1F-99B7-355F9E47661B}"/>
   </bookViews>
   <sheets>
     <sheet name="Consul" sheetId="1" r:id="rId1"/>
     <sheet name="Jaeger" sheetId="2" r:id="rId2"/>
+    <sheet name="Prometheus" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
   <si>
     <t>Using Amd64 version</t>
   </si>
@@ -158,6 +159,75 @@
   </si>
   <si>
     <t>Install service by nssm</t>
+  </si>
+  <si>
+    <t>Prometheus</t>
+  </si>
+  <si>
+    <t>Grafana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Windows Exporter </t>
+  </si>
+  <si>
+    <t>In case we want to monitor windows server</t>
+  </si>
+  <si>
+    <t>https://github.com/prometheus-community/windows_exporter/releases</t>
+  </si>
+  <si>
+    <t>Test in http://localhost:9182/metrics</t>
+  </si>
+  <si>
+    <t>Edit prometheus.yml</t>
+  </si>
+  <si>
+    <t>Add scrape job</t>
+  </si>
+  <si>
+    <t>Windows server exporter</t>
+  </si>
+  <si>
+    <t>- job_name: 'wmiexporter' 
+  scrape_interval: 30s 
+  static_configs: 
+     targets: ['WindowsIP:9182']</t>
+  </si>
+  <si>
+    <t>Download and install</t>
+  </si>
+  <si>
+    <t>http://localhost:3000</t>
+  </si>
+  <si>
+    <t>admin/admin</t>
+  </si>
+  <si>
+    <t>Install as service</t>
+  </si>
+  <si>
+    <t>Just run prometheus.exe</t>
+  </si>
+  <si>
+    <t>nssm install Prometheus PathOfPrometheus.exe</t>
+  </si>
+  <si>
+    <t>nssm start Prometheus</t>
+  </si>
+  <si>
+    <t>Add datasource of Prometheus with localhost:9090</t>
+  </si>
+  <si>
+    <t>localhost:9090</t>
+  </si>
+  <si>
+    <t>Add dashboard 2129</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>https://promcat.io/apps/mssql</t>
   </si>
 </sst>
 </file>
@@ -207,7 +277,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -215,6 +285,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -694,9 +766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EB05DD3-598B-41B8-8EB9-EA455645487F}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD22"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -847,4 +917,150 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5971F7B2-66DD-4D66-8011-3CA9B48C498C}">
+  <dimension ref="A1:D28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{7EA45889-1CC6-4917-8C2F-28786C8142F2}"/>
+    <hyperlink ref="B21" r:id="rId2" xr:uid="{E4389786-C265-45FD-A4A8-15538490D873}"/>
+    <hyperlink ref="B28" r:id="rId3" xr:uid="{5CA2780E-29BF-4583-8965-B102DCE3F20F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
+</worksheet>
 </file>
</xml_diff>